<commit_message>
New code for getting data from excel. Test data sheet also changed
</commit_message>
<xml_diff>
--- a/Desktop/infocampus/SourceCode/AppianJJ/testData/Testdata.xlsx
+++ b/Desktop/infocampus/SourceCode/AppianJJ/testData/Testdata.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
-    <sheet name="admin" sheetId="1" r:id="rId1"/>
-    <sheet name="Demand details" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
+    <sheet name="admin" sheetId="1" r:id="rId2"/>
+    <sheet name="Demand details" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
   <si>
     <t>Username</t>
   </si>
@@ -67,6 +68,36 @@
   </si>
   <si>
     <t>GS-16079-SOW-1.00</t>
+  </si>
+  <si>
+    <t>TestCaseName</t>
+  </si>
+  <si>
+    <t>MethodName</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Uname</t>
+  </si>
+  <si>
+    <t>SOW</t>
+  </si>
+  <si>
+    <t>TC_AddNewResource</t>
+  </si>
+  <si>
+    <t>TC_AddNewPosition</t>
+  </si>
+  <si>
+    <t>TC_OrderOwner_Approval</t>
+  </si>
+  <si>
+    <t>DemandID</t>
+  </si>
+  <si>
+    <t>GS-16075-SOW-2.00</t>
   </si>
 </sst>
 </file>
@@ -398,10 +429,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2">
+        <v>51745</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2">
+        <v>51745</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" display="Aug@20182018"/>
+    <hyperlink ref="C6" r:id="rId2" display="Aug@20182018"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,12 +619,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,7 +669,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2"/>
   <sheetViews>
@@ -524,18 +689,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
@@ -546,4 +699,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Code for getting test data from excel has been implemented.
</commit_message>
<xml_diff>
--- a/Desktop/infocampus/SourceCode/AppianJJ/testData/Testdata.xlsx
+++ b/Desktop/infocampus/SourceCode/AppianJJ/testData/Testdata.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
   <si>
     <t>Username</t>
   </si>
@@ -97,7 +97,16 @@
     <t>DemandID</t>
   </si>
   <si>
-    <t>GS-16075-SOW-2.00</t>
+    <t>date_from</t>
+  </si>
+  <si>
+    <t>date_to</t>
+  </si>
+  <si>
+    <t>empid</t>
+  </si>
+  <si>
+    <t>GS-16055-SOW-1.00</t>
   </si>
 </sst>
 </file>
@@ -121,15 +130,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -137,17 +152,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -429,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,121 +481,155 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="9">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="9">
+        <v>51741</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C9" s="10">
+        <v>43536</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="10">
+        <v>43544</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C11" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C12" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="2">
-        <v>51745</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="2">
-        <v>51745</v>
+      <c r="C13" s="9">
+        <v>51741</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" display="Aug@20182018"/>
-    <hyperlink ref="C6" r:id="rId2" display="Aug@20182018"/>
+    <hyperlink ref="C7" r:id="rId2" display="Aug@20182018"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -624,7 +696,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
New code for extend report
</commit_message>
<xml_diff>
--- a/Desktop/infocampus/SourceCode/AppianJJ/testData/Testdata.xlsx
+++ b/Desktop/infocampus/SourceCode/AppianJJ/testData/Testdata.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
   <si>
     <t>Username</t>
   </si>
@@ -106,7 +106,10 @@
     <t>empid</t>
   </si>
   <si>
-    <t>GS-16055-SOW-1.00</t>
+    <t>GS-16277-SOW-1.00</t>
+  </si>
+  <si>
+    <t>Welcome123</t>
   </si>
 </sst>
 </file>
@@ -144,7 +147,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -165,6 +168,174 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -172,7 +343,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -182,10 +353,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -470,7 +653,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +663,7 @@
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
@@ -492,144 +675,145 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>9</v>
+      <c r="C3" s="11" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="9">
-        <v>83</v>
+      <c r="C5" s="17">
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="9">
-        <v>51741</v>
+      <c r="C8" s="12">
+        <v>51787</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="10">
-        <v>43536</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="C9" s="13">
+        <v>43628</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="10">
-        <v>43544</v>
+      <c r="C10" s="21">
+        <v>43636</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="20" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="C12" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="9">
-        <v>51741</v>
+      <c r="C13" s="12">
+        <v>51787</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" display="Aug@20182018"/>
     <hyperlink ref="C7" r:id="rId2" display="Aug@20182018"/>
+    <hyperlink ref="C4" r:id="rId3" display="https://jnjtest.appiancloud.com/suite/tempo/tasks/assignedtome"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>